<commit_message>
codes equal, before improving random problem
</commit_message>
<xml_diff>
--- a/Code/QNN_EMG_modelo_full_RL/experiments/experimentsQNN/experiments_windowSize200_stride20_epoch1.xlsx
+++ b/Code/QNN_EMG_modelo_full_RL/experiments/experimentsQNN/experiments_windowSize200_stride20_epoch1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="1106">
   <si>
     <t>QNN - EMG - 5 gestures - Experience Replay</t>
   </si>
@@ -2951,6 +2951,321 @@
   </si>
   <si>
     <t>0%</t>
+  </si>
+  <si>
+    <t>26.67%</t>
+  </si>
+  <si>
+    <t>QNN - EMG - 5 gestures - Experience Replay</t>
+  </si>
+  <si>
+    <t>USER 8</t>
+  </si>
+  <si>
+    <t>VALIDATION RESULTS</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>numNeuronsLayers</t>
+  </si>
+  <si>
+    <t>RepTraining</t>
+  </si>
+  <si>
+    <t>Sampling type</t>
+  </si>
+  <si>
+    <t>learningRate</t>
+  </si>
+  <si>
+    <t>numEpochsToIncreaseMomentum</t>
+  </si>
+  <si>
+    <t>miniBatchSize</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Count Wins Recog</t>
+  </si>
+  <si>
+    <t>Count Wins Classif</t>
+  </si>
+  <si>
+    <t>Count Wins per window</t>
+  </si>
+  <si>
+    <t>Count Loses Recog</t>
+  </si>
+  <si>
+    <t>Count Loses Classif</t>
+  </si>
+  <si>
+    <t>Count Loses per window</t>
+  </si>
+  <si>
+    <t>Recognition</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Random Package</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>QNN - EMG - 5 gestures - Experience Replay</t>
+  </si>
+  <si>
+    <t>USER 8</t>
+  </si>
+  <si>
+    <t>TRAINING RESULTS</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>numNeuronsLayers</t>
+  </si>
+  <si>
+    <t>RepTraining</t>
+  </si>
+  <si>
+    <t>Sampling type</t>
+  </si>
+  <si>
+    <t>learningRate</t>
+  </si>
+  <si>
+    <t>numEpochsToIncreaseMomentum</t>
+  </si>
+  <si>
+    <t>miniBatchSize</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Count Wins Recog</t>
+  </si>
+  <si>
+    <t>Count Wins Classif</t>
+  </si>
+  <si>
+    <t>Count Wins per window</t>
+  </si>
+  <si>
+    <t>Count Loses Recog</t>
+  </si>
+  <si>
+    <t>Count Loses Classif</t>
+  </si>
+  <si>
+    <t>Count Loses per window</t>
+  </si>
+  <si>
+    <t>Recognition</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Random Package</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>13.33%</t>
+  </si>
+  <si>
+    <t>QNN - EMG - 5 gestures - Experience Replay</t>
+  </si>
+  <si>
+    <t>USER 8</t>
+  </si>
+  <si>
+    <t>VALIDATION RESULTS</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>numNeuronsLayers</t>
+  </si>
+  <si>
+    <t>RepTraining</t>
+  </si>
+  <si>
+    <t>Sampling type</t>
+  </si>
+  <si>
+    <t>learningRate</t>
+  </si>
+  <si>
+    <t>numEpochsToIncreaseMomentum</t>
+  </si>
+  <si>
+    <t>miniBatchSize</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Count Wins Recog</t>
+  </si>
+  <si>
+    <t>Count Wins Classif</t>
+  </si>
+  <si>
+    <t>Count Wins per window</t>
+  </si>
+  <si>
+    <t>Count Loses Recog</t>
+  </si>
+  <si>
+    <t>Count Loses Classif</t>
+  </si>
+  <si>
+    <t>Count Loses per window</t>
+  </si>
+  <si>
+    <t>Recognition</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Random Package</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>QNN - EMG - 5 gestures - Experience Replay</t>
+  </si>
+  <si>
+    <t>USER 8</t>
+  </si>
+  <si>
+    <t>TRAINING RESULTS</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>numNeuronsLayers</t>
+  </si>
+  <si>
+    <t>RepTraining</t>
+  </si>
+  <si>
+    <t>Sampling type</t>
+  </si>
+  <si>
+    <t>learningRate</t>
+  </si>
+  <si>
+    <t>numEpochsToIncreaseMomentum</t>
+  </si>
+  <si>
+    <t>miniBatchSize</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Count Wins Recog</t>
+  </si>
+  <si>
+    <t>Count Wins Classif</t>
+  </si>
+  <si>
+    <t>Count Wins per window</t>
+  </si>
+  <si>
+    <t>Count Loses Recog</t>
+  </si>
+  <si>
+    <t>Count Loses Classif</t>
+  </si>
+  <si>
+    <t>Count Loses per window</t>
+  </si>
+  <si>
+    <t>Recognition</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>QNN - EMG - 5 gestures - Experience Replay</t>
+  </si>
+  <si>
+    <t>USER 8</t>
+  </si>
+  <si>
+    <t>TRAINING RESULTS</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>numNeuronsLayers</t>
+  </si>
+  <si>
+    <t>RepTraining</t>
+  </si>
+  <si>
+    <t>Sampling type</t>
+  </si>
+  <si>
+    <t>learningRate</t>
+  </si>
+  <si>
+    <t>numEpochsToIncreaseMomentum</t>
+  </si>
+  <si>
+    <t>miniBatchSize</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Count Wins Recog</t>
+  </si>
+  <si>
+    <t>Count Wins Classif</t>
+  </si>
+  <si>
+    <t>Count Wins per window</t>
+  </si>
+  <si>
+    <t>Count Loses Recog</t>
+  </si>
+  <si>
+    <t>Count Loses Classif</t>
+  </si>
+  <si>
+    <t>Count Loses per window</t>
+  </si>
+  <si>
+    <t>Recognition</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Random Package</t>
+  </si>
+  <si>
+    <t>6.67%</t>
   </si>
   <si>
     <t>26.67%</t>
@@ -3037,7 +3352,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="274">
+  <borders count="303">
     <border>
       <left/>
       <right/>
@@ -3318,11 +3633,40 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -3597,6 +3941,35 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3632,63 +4005,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>958</v>
+        <v>1063</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>959</v>
+        <v>1064</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>960</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>961</v>
+        <v>1066</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>962</v>
+        <v>1067</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>963</v>
+        <v>1068</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>964</v>
+        <v>1069</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>965</v>
+        <v>1070</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>966</v>
+        <v>1071</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>967</v>
+        <v>1072</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>968</v>
+        <v>1073</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>969</v>
+        <v>1074</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>970</v>
+        <v>1075</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>971</v>
+        <v>1076</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>972</v>
+        <v>1077</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>973</v>
+        <v>1078</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>974</v>
+        <v>1079</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>975</v>
+        <v>1080</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>976</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="3">
@@ -3711,7 +4084,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>977</v>
+        <v>1082</v>
       </c>
       <c r="H3" s="0">
         <v>0.059999999999999998</v>
@@ -3726,89 +4099,89 @@
         <v>0</v>
       </c>
       <c r="L3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="0">
         <v>4</v>
       </c>
       <c r="N3" s="0">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="O3" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P3" s="0">
         <v>11</v>
       </c>
       <c r="Q3" s="0">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>978</v>
+        <v>1083</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>979</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>980</v>
+        <v>1085</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>981</v>
+        <v>1086</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>982</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>983</v>
+        <v>1088</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>984</v>
+        <v>1089</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>985</v>
+        <v>1090</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>986</v>
+        <v>1091</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>987</v>
+        <v>1092</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>988</v>
+        <v>1093</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>989</v>
+        <v>1094</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>990</v>
+        <v>1095</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>991</v>
+        <v>1096</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>992</v>
+        <v>1097</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>993</v>
+        <v>1098</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>994</v>
+        <v>1099</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>995</v>
+        <v>1100</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>996</v>
+        <v>1101</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>997</v>
+        <v>1102</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>998</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="7">
@@ -3831,7 +4204,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>999</v>
+        <v>1104</v>
       </c>
       <c r="H7" s="0">
         <v>0.059999999999999998</v>
@@ -3852,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O7" s="0">
         <v>5</v>
@@ -3861,13 +4234,13 @@
         <v>5</v>
       </c>
       <c r="Q7" s="0">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>1000</v>
+        <v>1105</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>1000</v>
+        <v>1105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>